<commit_message>
Bugfix: crater operator was only half ready. Before running with the crater operator the ripup_channel should be fixed and the operator itself should be fixed.
</commit_message>
<xml_diff>
--- a/Report/figures/Linkutil.xlsx
+++ b/Report/figures/Linkutil.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="14205" windowHeight="8805"/>
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>0.272727</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Link utilization</t>
   </si>
@@ -178,7 +175,7 @@
                 <c:formatCode>Standard</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.272727</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.4</c:v>
@@ -221,11 +218,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="128674048"/>
-        <c:axId val="133395200"/>
+        <c:axId val="62894464"/>
+        <c:axId val="62897152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="128674048"/>
+        <c:axId val="62894464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -250,12 +247,12 @@
         </c:title>
         <c:numFmt formatCode="Standard" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133395200"/>
+        <c:crossAx val="62897152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133395200"/>
+        <c:axId val="62897152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +266,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128674048"/>
+        <c:crossAx val="62894464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -301,9 +298,9 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
@@ -313,7 +310,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9306393" cy="6081947"/>
+    <xdr:ext cx="10247879" cy="7126741"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1"/>
@@ -623,23 +620,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F18:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="18" spans="6:7">
       <c r="G18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="6:7">
       <c r="F19">
         <v>9</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
+      <c r="G19" s="1">
+        <v>0.272727</v>
       </c>
     </row>
     <row r="20" spans="6:7">

</xml_diff>